<commit_message>
Transcribed liv_002704, marked such
</commit_message>
<xml_diff>
--- a/DL-Transcribed-Letters.xlsx
+++ b/DL-Transcribed-Letters.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2410" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="1052">
   <si>
     <t>liv_000043</t>
   </si>
@@ -3644,8 +3644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A705" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B721" sqref="B721"/>
+    <sheetView tabSelected="1" topLeftCell="A713" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B722" sqref="B722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9418,82 +9418,85 @@
         <v>964</v>
       </c>
     </row>
-    <row r="721" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" s="3" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="722" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B721" s="6" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" s="3" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="723" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" s="3" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="724" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" s="3" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="725" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" s="3" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="726" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" s="3" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="727" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" s="3" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="728" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" s="3" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="729" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" s="3" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="730" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" s="3" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="731" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" s="3" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="732" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" s="3" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="733" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" s="3" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="734" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" s="3" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="735" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" s="3" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="736" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" s="3" t="s">
         <v>734</v>
       </c>

</xml_diff>

<commit_message>
Proof 1318, corrected 2705
moved appropriate files to appropriate folders
</commit_message>
<xml_diff>
--- a/DL-Transcribed-Letters.xlsx
+++ b/DL-Transcribed-Letters.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2411" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="1052">
   <si>
     <t>liv_000043</t>
   </si>
@@ -3645,7 +3645,7 @@
   <dimension ref="A1:D977"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A713" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B722" sqref="B722"/>
+      <selection activeCell="B723" sqref="B723"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9429,6 +9429,9 @@
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" s="3" t="s">
         <v>720</v>
+      </c>
+      <c r="B722" s="6" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>